<commit_message>
-Revive Phantom Knight Prototype.xlsx
</commit_message>
<xml_diff>
--- a/企劃/Phantom Knight Prototype.xlsx
+++ b/企劃/Phantom Knight Prototype.xlsx
@@ -13,6 +13,22 @@
   <definedNames/>
   <calcPr/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="A15">
+      <text>
+        <t xml:space="preserve">為了讓玩家可以穿梭在萬軍之中，不會因為敵人堵住所有下落空間導致玩家受到傷害。
+	-Bridge Lin</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -108,15 +124,6 @@
     <t>https://cowlevel.net/article/2017835</t>
   </si>
   <si>
-    <t>跳殺</t>
-  </si>
-  <si>
-    <t>跳到敵人頭上，對其造成傷害，玩家角色向上反彈</t>
-  </si>
-  <si>
-    <t>像是空洞騎士向下砍，鏟子騎士向下鏟</t>
-  </si>
-  <si>
     <t>攻擊</t>
   </si>
   <si>
@@ -144,6 +151,15 @@
     <t>0.5秒(暫定)未攻擊到敵人就重置</t>
   </si>
   <si>
+    <t>跳殺</t>
+  </si>
+  <si>
+    <t>跳到敵人頭上，對其造成傷害，玩家角色向上反彈</t>
+  </si>
+  <si>
+    <t>像是空洞騎士向下砍，鏟子騎士向下鏟</t>
+  </si>
+  <si>
     <t>敵人</t>
   </si>
   <si>
@@ -159,7 +175,7 @@
     <t>AI</t>
   </si>
   <si>
-    <t>當玩家在其前方一定距離，會開始暴衝</t>
+    <t>當玩家在其前方一定距離，會開始攻擊</t>
   </si>
   <si>
     <t>扣血、顯示受傷動畫、被擊退</t>
@@ -304,7 +320,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/m/d"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -328,7 +344,6 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
-    <font/>
     <font>
       <sz val="11.0"/>
       <color rgb="FFFFFFFF"/>
@@ -404,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -445,10 +460,7 @@
     <xf borderId="1" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
     <xf borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
@@ -460,10 +472,10 @@
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -7102,40 +7114,40 @@
       <c r="Z10" s="6"/>
     </row>
     <row r="11">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="15"/>
-      <c r="Z11" s="15"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
     </row>
     <row r="12">
       <c r="A12" s="11" t="s">
@@ -7147,9 +7159,7 @@
       <c r="C12" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>34</v>
-      </c>
+      <c r="D12" s="12"/>
       <c r="E12" s="12"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -7178,10 +7188,10 @@
         <v>22</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
@@ -7212,10 +7222,10 @@
         <v>22</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
@@ -7246,47 +7256,49 @@
         <v>22</v>
       </c>
       <c r="B15" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="D15" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="6"/>
-      <c r="T15" s="6"/>
-      <c r="U15" s="6"/>
-      <c r="V15" s="6"/>
-      <c r="W15" s="6"/>
-      <c r="X15" s="6"/>
-      <c r="Y15" s="6"/>
-      <c r="Z15" s="6"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="14"/>
+      <c r="V15" s="14"/>
+      <c r="W15" s="14"/>
+      <c r="X15" s="14"/>
+      <c r="Y15" s="14"/>
+      <c r="Z15" s="14"/>
     </row>
     <row r="16">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="16" t="s">
-        <v>35</v>
+      <c r="B16" s="15" t="s">
+        <v>32</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
@@ -7310,17 +7322,17 @@
       <c r="Z16" s="6"/>
     </row>
     <row r="17">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -7344,17 +7356,17 @@
       <c r="Z17" s="6"/>
     </row>
     <row r="18">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
@@ -7378,17 +7390,17 @@
       <c r="Z18" s="6"/>
     </row>
     <row r="19">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>37</v>
+      <c r="B19" s="15" t="s">
+        <v>34</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -7412,17 +7424,17 @@
       <c r="Z19" s="6"/>
     </row>
     <row r="20">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
@@ -7446,17 +7458,17 @@
       <c r="Z20" s="6"/>
     </row>
     <row r="21">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
@@ -7480,17 +7492,17 @@
       <c r="Z21" s="6"/>
     </row>
     <row r="22">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
@@ -7514,11 +7526,11 @@
       <c r="Z22" s="6"/>
     </row>
     <row r="23">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
@@ -7542,11 +7554,11 @@
       <c r="Z23" s="6"/>
     </row>
     <row r="24">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
@@ -7570,11 +7582,11 @@
       <c r="Z24" s="6"/>
     </row>
     <row r="25">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
@@ -7598,11 +7610,11 @@
       <c r="Z25" s="6"/>
     </row>
     <row r="26">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
@@ -7626,11 +7638,11 @@
       <c r="Z26" s="6"/>
     </row>
     <row r="27">
-      <c r="A27" s="18"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
@@ -7654,11 +7666,11 @@
       <c r="Z27" s="6"/>
     </row>
     <row r="28">
-      <c r="A28" s="18"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
@@ -34899,9 +34911,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E10"/>
+    <hyperlink r:id="rId2" ref="E10"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -34920,170 +34933,170 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="19" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="19" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="19" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="19" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="19" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="19" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="19" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="19" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="19" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>

<commit_message>
-Add the flowchart of the whole game and the flowchart of Challenge Mode to Phantom Knight Prototype.xlsx
</commit_message>
<xml_diff>
--- a/企劃/Phantom Knight Prototype.xlsx
+++ b/企劃/Phantom Knight Prototype.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="111">
   <si>
     <t>日期</t>
   </si>
@@ -331,6 +331,21 @@
     <t>小怪偵測到玩家開始暴衝的距離</t>
   </si>
   <si>
+    <t>流程圖原檔：</t>
+  </si>
+  <si>
+    <t>https://app.diagrams.net/#G198RaeA3XA_b2Xfwl_2D2yFxYfitIzsvj</t>
+  </si>
+  <si>
+    <t>遊戲整體流程圖</t>
+  </si>
+  <si>
+    <t>故事模式</t>
+  </si>
+  <si>
+    <t>挑戰模式</t>
+  </si>
+  <si>
     <t>1.左下角放玩家頭像、血條、技能(如果有的話)</t>
   </si>
   <si>
@@ -362,7 +377,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/m/d"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -377,6 +392,10 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+    </font>
+    <font/>
     <font>
       <b/>
       <color theme="0"/>
@@ -395,6 +414,10 @@
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF1155CC"/>
     </font>
   </fonts>
   <fills count="8">
@@ -461,7 +484,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -484,7 +507,13 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
@@ -499,7 +528,7 @@
     <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -514,13 +543,22 @@
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="7" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -548,18 +586,74 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>942975</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>-19050</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="5438775" cy="10039350"/>
+    <xdr:ext cx="10944225" cy="6438900"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image7.png" title="圖片"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>-133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4562475" cy="8439150"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="0" name="image5.png" title="圖片"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>-180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4562475" cy="14411325"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image6.png" title="圖片"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -588,7 +682,7 @@
     <xdr:ext cx="5133975" cy="2886075"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="圖片"/>
+        <xdr:cNvPr id="0" name="image8.png" title="圖片"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -616,7 +710,7 @@
     <xdr:ext cx="3048000" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="圖片"/>
+        <xdr:cNvPr id="0" name="image1.png" title="圖片"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -672,7 +766,7 @@
     <xdr:ext cx="3048000" cy="342900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="圖片"/>
+        <xdr:cNvPr id="0" name="image2.png" title="圖片"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -7030,7 +7124,7 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="6"/>
@@ -7061,7 +7155,7 @@
     </row>
     <row r="4">
       <c r="A4" s="7"/>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="6"/>
@@ -7091,7 +7185,7 @@
     </row>
     <row r="5">
       <c r="A5" s="7"/>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="9" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="6"/>
@@ -7121,7 +7215,7 @@
     </row>
     <row r="6">
       <c r="A6" s="7"/>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="6"/>
@@ -7151,7 +7245,7 @@
     </row>
     <row r="7">
       <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -7206,19 +7300,19 @@
       <c r="Z8" s="6"/>
     </row>
     <row r="9">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F9" s="6"/>
@@ -7244,17 +7338,17 @@
       <c r="Z9" s="6"/>
     </row>
     <row r="10">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
@@ -7278,17 +7372,17 @@
       <c r="Z10" s="6"/>
     </row>
     <row r="11">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -7312,19 +7406,19 @@
       <c r="Z11" s="6"/>
     </row>
     <row r="12">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="10"/>
+      <c r="E12" s="12"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
@@ -7348,17 +7442,17 @@
       <c r="Z12" s="6"/>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
@@ -7382,19 +7476,19 @@
       <c r="Z13" s="6"/>
     </row>
     <row r="14">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="15" t="s">
         <v>32</v>
       </c>
       <c r="F14" s="6"/>
@@ -7420,19 +7514,19 @@
       <c r="Z14" s="6"/>
     </row>
     <row r="15">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="12"/>
+      <c r="E15" s="14"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
@@ -7456,17 +7550,17 @@
       <c r="Z15" s="6"/>
     </row>
     <row r="16">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
@@ -7490,17 +7584,17 @@
       <c r="Z16" s="6"/>
     </row>
     <row r="17">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -7524,17 +7618,17 @@
       <c r="Z17" s="6"/>
     </row>
     <row r="18">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
@@ -7558,53 +7652,53 @@
       <c r="Z18" s="6"/>
     </row>
     <row r="19">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="14"/>
-      <c r="T19" s="14"/>
-      <c r="U19" s="14"/>
-      <c r="V19" s="14"/>
-      <c r="W19" s="14"/>
-      <c r="X19" s="14"/>
-      <c r="Y19" s="14"/>
-      <c r="Z19" s="14"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="16"/>
+      <c r="T19" s="16"/>
+      <c r="U19" s="16"/>
+      <c r="V19" s="16"/>
+      <c r="W19" s="16"/>
+      <c r="X19" s="16"/>
+      <c r="Y19" s="16"/>
+      <c r="Z19" s="16"/>
     </row>
     <row r="20">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
@@ -7628,17 +7722,17 @@
       <c r="Z20" s="6"/>
     </row>
     <row r="21">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
@@ -7662,17 +7756,17 @@
       <c r="Z21" s="6"/>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
@@ -7696,17 +7790,17 @@
       <c r="Z22" s="6"/>
     </row>
     <row r="23">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
@@ -7730,17 +7824,17 @@
       <c r="Z23" s="6"/>
     </row>
     <row r="24">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
@@ -7764,17 +7858,17 @@
       <c r="Z24" s="6"/>
     </row>
     <row r="25">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
@@ -7798,17 +7892,17 @@
       <c r="Z25" s="6"/>
     </row>
     <row r="26">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
@@ -7832,17 +7926,17 @@
       <c r="Z26" s="6"/>
     </row>
     <row r="27">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
@@ -7866,11 +7960,11 @@
       <c r="Z27" s="6"/>
     </row>
     <row r="28">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
@@ -7894,11 +7988,11 @@
       <c r="Z28" s="6"/>
     </row>
     <row r="29">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
@@ -7922,11 +8016,11 @@
       <c r="Z29" s="6"/>
     </row>
     <row r="30">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
+      <c r="A30" s="19"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
@@ -7950,11 +8044,11 @@
       <c r="Z30" s="6"/>
     </row>
     <row r="31">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
+      <c r="A31" s="19"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
@@ -7978,11 +8072,11 @@
       <c r="Z31" s="6"/>
     </row>
     <row r="32">
-      <c r="A32" s="17"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
+      <c r="A32" s="19"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
@@ -35245,170 +35339,170 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="21" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="21" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="21" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="21" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="21" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="21" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="21" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="21" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="21" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="21" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="21" t="s">
         <v>97</v>
       </c>
     </row>
@@ -41360,8 +41454,35 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData/>
-  <drawing r:id="rId1"/>
+  <sheetData>
+    <row r="2">
+      <c r="B2" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="B83" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" location="G198RaeA3XA_b2Xfwl_2D2yFxYfitIzsvj" ref="C2"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -41376,43 +41497,43 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="17">
-      <c r="C17" s="20" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="C18" s="20" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="C19" s="20" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="C20" s="20" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="C21" s="20" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="C22" s="20" t="s">
+      <c r="C17" s="24" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="26">
-      <c r="C26" s="20" t="s">
+    <row r="18">
+      <c r="C18" s="25" t="s">
         <v>104</v>
       </c>
     </row>
+    <row r="19">
+      <c r="C19" s="24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" s="24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="C22" s="24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="C26" s="24" t="s">
+        <v>109</v>
+      </c>
+    </row>
     <row r="30">
-      <c r="C30" s="20" t="s">
-        <v>105</v>
+      <c r="C30" s="24" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>